<commit_message>
TEX: More ETD fixes
</commit_message>
<xml_diff>
--- a/DOC/AreaEstimates.xlsx
+++ b/DOC/AreaEstimates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="2040" windowWidth="51200" windowHeight="27040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Manager" sheetId="2" r:id="rId1"/>
@@ -871,6 +871,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -879,12 +885,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="219">
@@ -1445,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:AF68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="U32" sqref="U32:W37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J8" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1543,10 +1543,10 @@
         <f>X59/X62</f>
         <v>0.51355879341490751</v>
       </c>
-      <c r="N13" s="31" t="s">
+      <c r="N13" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="O13" s="33"/>
+      <c r="O13" s="35"/>
     </row>
     <row r="14" spans="3:17">
       <c r="C14" t="s">
@@ -1916,15 +1916,15 @@
         <f>SUM(N29:N31)</f>
         <v>2495</v>
       </c>
-      <c r="Q32" s="31" t="s">
+      <c r="Q32" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="R32" s="32"/>
-      <c r="S32" s="33"/>
-      <c r="V32" s="31" t="s">
+      <c r="R32" s="34"/>
+      <c r="S32" s="35"/>
+      <c r="V32" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="W32" s="33"/>
+      <c r="W32" s="35"/>
     </row>
     <row r="33" spans="5:32">
       <c r="E33" t="s">
@@ -2003,22 +2003,22 @@
         <f>I26+I27</f>
         <v>0.20611733011287103</v>
       </c>
-      <c r="R34" s="35">
+      <c r="R34" s="32">
         <f>(H26+H27)/$S$46</f>
         <v>0.99399999999999999</v>
       </c>
-      <c r="S34" s="35">
+      <c r="S34" s="32">
         <f>(K26+K27)/$S$46</f>
         <v>0.36347834385916716</v>
       </c>
       <c r="U34" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="V34" s="34">
+      <c r="V34" s="31">
         <f>R43</f>
         <v>4.822496000000001</v>
       </c>
-      <c r="W34" s="34">
+      <c r="W34" s="31">
         <f>S43</f>
         <v>1.9751604246322549</v>
       </c>
@@ -2059,22 +2059,22 @@
         <f>I29</f>
         <v>6.9466102201017899E-2</v>
       </c>
-      <c r="R35" s="35">
+      <c r="R35" s="32">
         <f>H29/$S$46</f>
         <v>0.33500000000000002</v>
       </c>
-      <c r="S35" s="35">
+      <c r="S35" s="32">
         <f>K29/$S$46</f>
         <v>0.12250024667285814</v>
       </c>
       <c r="U35" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="V35" s="34">
+      <c r="V35" s="31">
         <f>P19</f>
         <v>6.661495908618436</v>
       </c>
-      <c r="W35" s="34">
+      <c r="W35" s="31">
         <f>N19</f>
         <v>2.43432</v>
       </c>
@@ -2119,11 +2119,11 @@
         <f>I30</f>
         <v>0.47074709859790448</v>
       </c>
-      <c r="R36" s="35">
+      <c r="R36" s="32">
         <f>H30/$S$46</f>
         <v>2.2701760000000002</v>
       </c>
-      <c r="S36" s="35">
+      <c r="S36" s="32">
         <f>K30/$S$46</f>
         <v>0.83014065668896242</v>
       </c>
@@ -2172,11 +2172,11 @@
         <f>I31</f>
         <v>6.6563041213512669E-2</v>
       </c>
-      <c r="R37" s="35">
+      <c r="R37" s="32">
         <f>H31/$S$46</f>
         <v>0.32100000000000001</v>
       </c>
-      <c r="S37" s="35">
+      <c r="S37" s="32">
         <f>K31/$S$46</f>
         <v>0.11738083337906706</v>
       </c>
@@ -2230,11 +2230,11 @@
         <f>I35+I36+I37+I32</f>
         <v>1.732920048041512E-2</v>
       </c>
-      <c r="R38" s="35">
+      <c r="R38" s="32">
         <f>(H35+H36+H37+H32)/$S$46</f>
         <v>8.3570000000000005E-2</v>
       </c>
-      <c r="S38" s="35">
+      <c r="S38" s="32">
         <f>(K35+K36+K37+K32)/$S$46</f>
         <v>3.0559240640151503E-2</v>
       </c>
@@ -2284,11 +2284,11 @@
         <f>I33+I34</f>
         <v>1.6174196930386256E-2</v>
       </c>
-      <c r="R39" s="35">
+      <c r="R39" s="32">
         <f>(H33+H34)/$S$46</f>
         <v>7.8E-2</v>
       </c>
-      <c r="S39" s="35">
+      <c r="S39" s="32">
         <f>(K33+K34)/$S$46</f>
         <v>2.852244549397891E-2</v>
       </c>
@@ -2309,11 +2309,11 @@
         <f>I28</f>
         <v>1.5966835431278741E-2</v>
       </c>
-      <c r="R40" s="35">
+      <c r="R40" s="32">
         <f>H28/$S$46</f>
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="S40" s="35">
+      <c r="S40" s="32">
         <f>K28/$S$46</f>
         <v>2.8156773115850978E-2</v>
       </c>
@@ -2359,11 +2359,11 @@
         <f>I41</f>
         <v>6.9206900327133503E-2</v>
       </c>
-      <c r="R41" s="35">
+      <c r="R41" s="32">
         <f>H41/$S$46</f>
         <v>0.33374999999999999</v>
       </c>
-      <c r="S41" s="35">
+      <c r="S41" s="32">
         <f>K41/$S$46</f>
         <v>0.33374999999999999</v>
       </c>
@@ -2394,11 +2394,11 @@
         <f>I39</f>
         <v>6.8429294705480315E-2</v>
       </c>
-      <c r="R42" s="35">
+      <c r="R42" s="32">
         <f>H39/$S$46</f>
         <v>0.33</v>
       </c>
-      <c r="S42" s="35">
+      <c r="S42" s="32">
         <f>K39/$S$46</f>
         <v>0.12067188478221846</v>
       </c>
@@ -2409,11 +2409,11 @@
         <f>SUM(Q34:Q42)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="R43" s="35">
+      <c r="R43" s="32">
         <f>SUM(R34:R42)</f>
         <v>4.822496000000001</v>
       </c>
-      <c r="S43" s="35">
+      <c r="S43" s="32">
         <f>SUM(S34:S42)</f>
         <v>1.9751604246322549</v>
       </c>
@@ -2789,8 +2789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:R75"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61:M72"/>
+    <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2954,7 +2954,7 @@
       </c>
       <c r="Q19">
         <f>H42/P19/1000000</f>
-        <v>0.53625027940096437</v>
+        <v>0.54620892805824317</v>
       </c>
     </row>
     <row r="22" spans="3:18">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="Q22">
         <f>(H42-H41)/(P19*1000000-H41)</f>
-        <v>0.5268259307828268</v>
+        <v>0.532233975585371</v>
       </c>
     </row>
     <row r="25" spans="3:18">
@@ -2994,7 +2994,7 @@
       </c>
       <c r="I26" s="9">
         <f>H26/$H$42</f>
-        <v>0.16375139560848531</v>
+        <v>0.16076582995359714</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>41</v>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="I27" s="9">
         <f t="shared" ref="I27:I33" si="1">H27/$H$42</f>
-        <v>3.1261630070710832E-2</v>
+        <v>3.0691658445686727E-2</v>
       </c>
       <c r="L27" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3052,7 +3052,7 @@
       </c>
       <c r="I28" s="9">
         <f t="shared" si="1"/>
-        <v>9.5273539263118715E-3</v>
+        <v>9.3536482882092872E-3</v>
       </c>
     </row>
     <row r="29" spans="3:18">
@@ -3071,7 +3071,7 @@
       </c>
       <c r="I29" s="9">
         <f t="shared" si="1"/>
-        <v>0.17863788611834761</v>
+        <v>0.17538090540392415</v>
       </c>
       <c r="L29">
         <f>4100*2</f>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="I30" s="9">
         <f t="shared" si="1"/>
-        <v>0.4001488649050986</v>
+        <v>0.39285322810479006</v>
       </c>
       <c r="L30">
         <f>2700*2</f>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="I31" s="9">
         <f t="shared" si="1"/>
-        <v>5.0614067733531819E-3</v>
+        <v>4.9691256531111845E-3</v>
       </c>
       <c r="L31">
         <f>L29+L30</f>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="I32" s="9">
         <f t="shared" si="1"/>
-        <v>1.9054707852623743E-2</v>
+        <v>1.8707296576418574E-2</v>
       </c>
       <c r="N32">
         <f>SUM(N29:N31)</f>
@@ -3190,7 +3190,7 @@
       </c>
       <c r="I33" s="9">
         <f t="shared" si="1"/>
-        <v>0.15094901377000372</v>
+        <v>0.14819686506631591</v>
       </c>
       <c r="J33" t="s">
         <v>108</v>
@@ -3261,13 +3261,13 @@
       </c>
       <c r="I39" s="9">
         <f>H39/$H$42</f>
-        <v>4.4659471529586896E-3</v>
+        <v>4.3845226350981035E-3</v>
       </c>
       <c r="M39" t="s">
         <v>38</v>
       </c>
       <c r="N39" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="5:14">
@@ -3285,22 +3285,22 @@
       </c>
       <c r="F41">
         <f>N42</f>
-        <v>124750</v>
+        <v>187125</v>
       </c>
       <c r="G41">
         <v>1</v>
       </c>
       <c r="H41">
         <f>F41*G41</f>
-        <v>124750</v>
+        <v>187125</v>
       </c>
       <c r="I41" s="9">
         <f>H41/$H$42</f>
-        <v>3.7141793822106438E-2</v>
+        <v>5.4696919872848845E-2</v>
       </c>
       <c r="N41">
         <f>N38+N39*N38</f>
-        <v>4990</v>
+        <v>7485</v>
       </c>
     </row>
     <row r="42" spans="5:14">
@@ -3309,14 +3309,14 @@
       </c>
       <c r="H42" s="2">
         <f>H40+H41</f>
-        <v>3358750</v>
+        <v>3421125</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="N42" s="2">
         <f>N41/N27*1000000</f>
-        <v>124750</v>
+        <v>187125</v>
       </c>
     </row>
     <row r="46" spans="5:14">
@@ -3500,17 +3500,17 @@
     </row>
     <row r="60" spans="5:18">
       <c r="J60" s="1"/>
-      <c r="Q60" s="31" t="s">
+      <c r="Q60" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="R60" s="33"/>
+      <c r="R60" s="35"/>
     </row>
     <row r="61" spans="5:18">
-      <c r="K61" s="31" t="s">
+      <c r="K61" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="L61" s="32"/>
-      <c r="M61" s="33"/>
+      <c r="L61" s="34"/>
+      <c r="M61" s="35"/>
       <c r="P61" s="24"/>
       <c r="Q61" s="22" t="s">
         <v>93</v>
@@ -3533,13 +3533,13 @@
       <c r="P62" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q62" s="34">
+      <c r="Q62" s="31">
         <f>L72</f>
-        <v>3.3587500000000006</v>
-      </c>
-      <c r="R62" s="34">
+        <v>3.4211250000000004</v>
+      </c>
+      <c r="R62" s="31">
         <f>M72</f>
-        <v>1.3065552563561116</v>
+        <v>1.3689302563561117</v>
       </c>
     </row>
     <row r="63" spans="5:18">
@@ -3548,24 +3548,24 @@
       </c>
       <c r="K63" s="21">
         <f>I27</f>
-        <v>3.1261630070710832E-2</v>
-      </c>
-      <c r="L63" s="34">
+        <v>3.0691658445686727E-2</v>
+      </c>
+      <c r="L63" s="31">
         <f>H27/$M$75</f>
         <v>0.105</v>
       </c>
-      <c r="M63" s="34">
+      <c r="M63" s="31">
         <f>IF(EXACT(J63,"TSV"),L63,L63/Manager!$O$19)</f>
         <v>3.8370300531042588E-2</v>
       </c>
       <c r="P63" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="Q63" s="34">
+      <c r="Q63" s="31">
         <f>Manager!P19</f>
         <v>6.661495908618436</v>
       </c>
-      <c r="R63" s="34">
+      <c r="R63" s="31">
         <f>Manager!N19</f>
         <v>2.43432</v>
       </c>
@@ -3576,13 +3576,13 @@
       </c>
       <c r="K64" s="21">
         <f>I31+I28</f>
-        <v>1.4588760699665054E-2</v>
-      </c>
-      <c r="L64" s="34">
+        <v>1.4322773941320472E-2</v>
+      </c>
+      <c r="L64" s="31">
         <f>(H31+H28)/$M$75</f>
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="M64" s="34">
+      <c r="M64" s="31">
         <f>IF(EXACT(J64,"TSV"),L64,L64/Manager!$O$19)</f>
         <v>1.7906140247819877E-2</v>
       </c>
@@ -3591,11 +3591,11 @@
       </c>
       <c r="Q64" s="23">
         <f>Q62/Q63</f>
-        <v>0.50420356719795545</v>
+        <v>0.51356707966657389</v>
       </c>
       <c r="R64" s="23">
         <f>R62/R63</f>
-        <v>0.5367228862089255</v>
+        <v>0.56234605818302918</v>
       </c>
     </row>
     <row r="65" spans="10:18">
@@ -3604,13 +3604,13 @@
       </c>
       <c r="K65" s="21">
         <f>I33</f>
-        <v>0.15094901377000372</v>
-      </c>
-      <c r="L65" s="34">
+        <v>0.14819686506631591</v>
+      </c>
+      <c r="L65" s="31">
         <f>H33/$M$75</f>
         <v>0.50700000000000001</v>
       </c>
-      <c r="M65" s="34">
+      <c r="M65" s="31">
         <f>IF(EXACT(J65,"TSV"),L65,L65/Manager!$O$19)</f>
         <v>0.18527373684989135</v>
       </c>
@@ -3619,11 +3619,11 @@
       </c>
       <c r="Q65" s="23">
         <f>(L72-L70)/(Q63-L70)</f>
-        <v>0.49474158017005093</v>
+        <v>0.49950799014233532</v>
       </c>
       <c r="R65" s="23">
         <f>(M72-M70)/(R63-M70)</f>
-        <v>0.51169925845768338</v>
+        <v>0.52590240560169976</v>
       </c>
     </row>
     <row r="66" spans="10:18">
@@ -3632,13 +3632,13 @@
       </c>
       <c r="K66" s="21">
         <f>I29</f>
-        <v>0.17863788611834761</v>
-      </c>
-      <c r="L66" s="34">
+        <v>0.17538090540392415</v>
+      </c>
+      <c r="L66" s="31">
         <f>H29/$M$75</f>
         <v>0.6</v>
       </c>
-      <c r="M66" s="34">
+      <c r="M66" s="31">
         <f>IF(EXACT(J66,"TSV"),L66,L66/Manager!$O$19)</f>
         <v>0.21925886017738622</v>
       </c>
@@ -3649,13 +3649,13 @@
       </c>
       <c r="K67" s="21">
         <f>I30</f>
-        <v>0.4001488649050986</v>
-      </c>
-      <c r="L67" s="34">
+        <v>0.39285322810479006</v>
+      </c>
+      <c r="L67" s="31">
         <f>H30/$M$75</f>
         <v>1.3440000000000001</v>
       </c>
-      <c r="M67" s="34">
+      <c r="M67" s="31">
         <f>IF(EXACT(J67,"TSV"),L67,L67/Manager!$O$19)</f>
         <v>0.49113984679734518</v>
       </c>
@@ -3666,13 +3666,13 @@
       </c>
       <c r="K68" s="21">
         <f>I32</f>
-        <v>1.9054707852623743E-2</v>
-      </c>
-      <c r="L68" s="34">
+        <v>1.8707296576418574E-2</v>
+      </c>
+      <c r="L68" s="31">
         <f>H32/$M$75</f>
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="M68" s="34">
+      <c r="M68" s="31">
         <f>IF(EXACT(J68,"TSV"),L68,L68/Manager!$O$19)</f>
         <v>2.3387611752254532E-2</v>
       </c>
@@ -3683,13 +3683,13 @@
       </c>
       <c r="K69" s="21">
         <f>I26</f>
-        <v>0.16375139560848531</v>
-      </c>
-      <c r="L69" s="34">
+        <v>0.16076582995359714</v>
+      </c>
+      <c r="L69" s="31">
         <f>H26/$M$75</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="M69" s="34">
+      <c r="M69" s="31">
         <f>IF(EXACT(J69,"TSV"),L69,L69/Manager!$O$19)</f>
         <v>0.20098728849593739</v>
       </c>
@@ -3700,15 +3700,15 @@
       </c>
       <c r="K70" s="21">
         <f>I41</f>
-        <v>3.7141793822106438E-2</v>
-      </c>
-      <c r="L70" s="34">
+        <v>5.4696919872848845E-2</v>
+      </c>
+      <c r="L70" s="31">
         <f>H41/$M$75</f>
-        <v>0.12475</v>
-      </c>
-      <c r="M70" s="34">
+        <v>0.18712500000000001</v>
+      </c>
+      <c r="M70" s="31">
         <f>IF(EXACT(J70,"TSV"),L70,L70/Manager!$O$19)</f>
-        <v>0.12475</v>
+        <v>0.18712500000000001</v>
       </c>
     </row>
     <row r="71" spans="10:18">
@@ -3717,13 +3717,13 @@
       </c>
       <c r="K71" s="21">
         <f>I39</f>
-        <v>4.4659471529586896E-3</v>
-      </c>
-      <c r="L71" s="34">
+        <v>4.3845226350981035E-3</v>
+      </c>
+      <c r="L71" s="31">
         <f>H39/$M$75</f>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M71" s="34">
+      <c r="M71" s="31">
         <f>IF(EXACT(J71,"TSV"),L71,L71/Manager!$O$19)</f>
         <v>5.4814715044346554E-3</v>
       </c>
@@ -3736,13 +3736,13 @@
         <f>SUM(K63:K71)</f>
         <v>1</v>
       </c>
-      <c r="L72" s="34">
+      <c r="L72" s="31">
         <f>SUM(L63:L71)</f>
-        <v>3.3587500000000006</v>
-      </c>
-      <c r="M72" s="34">
+        <v>3.4211250000000004</v>
+      </c>
+      <c r="M72" s="31">
         <f>SUM(M63:M71)</f>
-        <v>1.3065552563561116</v>
+        <v>1.3689302563561117</v>
       </c>
     </row>
     <row r="74" spans="10:18">

</xml_diff>